<commit_message>
made the generic for all contents
</commit_message>
<xml_diff>
--- a/Utils/excel.xlsx
+++ b/Utils/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhisheksingh29\Desktop\GenAi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Generative\Generative-AI-\Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C69FE1-3E78-44CC-BB66-BCE4C626B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B06202-CE6F-4C16-B043-245DCD074730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADA0E984-BFC4-4595-A46A-2DBF17786137}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
   <si>
     <t>fs-general_fields-assumptions</t>
   </si>
@@ -251,102 +251,305 @@
     <t>tut-test_case5-expected_results</t>
   </si>
   <si>
-    <t>1.The Profit Center information is going to be entered in the hierarchical format specified in this specification
-2.The data will be cleansed and signed off by the business prior to load
-3.Error found at the time of actual upload will be stored separately in error log file. This file will be rectified as per Error Management available in SM35 transaction code. This will be done till all required data is successfully uploaded into SAP S/4HANA.</t>
-  </si>
-  <si>
-    <t>1.The Profit Center groups (Hierarchy) must be created prior to this upload as the Profit Center will have to be assigned to Profit Center groups.                                             2.Profit Center groups (Hierarchy) would be created manually in the system and the same will be used while creating the Profit Center master data using this upload. The user ID performing the load should have the controlling area assigned as a predetermined value.</t>
-  </si>
-  <si>
-    <t>This document contains specification to upload Profit Center master data in SAP S/4HANA using an upload program as opposed to creating Profit Centers manually in SAP S/4HANA. Manual creation would be a large undertaking due to volume, in addition to the risk of errors associated with creating master data manually. With the help of an upload program, data load would be efficient and consistent.
-Profit Center master data is prerequisite for transaction processing in SAP S/4HANA in addition to the cost center master data.
-A Profit Center is an organizational unit in accounting that reflects a management-oriented structure of the organization for the purpose of internal control.
-Requirements
-1.Profit Centers must be created and activated through this upload.
-2.Profit Center groups (Hierarchy) should be created prior to executing the upload.</t>
-  </si>
-  <si>
-    <t>Upload should show a summary of the process status including Profit Centers created, Profit Centers activated, and account of errors.  The error log should contain a detailed overview of each error.  Log of all data in SAP created from upload should be extractable. 
-Automated Load Process
-Create an error file in the same format. Append the error message at the end of the data columns. This will be used for manual review and correction. The corrected file shall be renamed and resubmitted for execution. Use the following naming convention for the file will be as per upload strategy.
-Manual Correction
-Scenario 1: Profit Center Master Data was not created:
-Determine which fields were incorrect and which Profit Centers failed to load. Next, manually create them in SAP. Alternatively, make the correction and re-submit the EAP data file for execution through the upload.
-Scenario 2: Master Data was created with incorrect parameters:
-Profit Centers (prior to any postings being made) may be individually deleted using transaction KE54 – Delete Profit Center.</t>
-  </si>
-  <si>
-    <t>Profit Centers are organizational units in SAP S/4HANA by which one can track profitability associated with the business unit below the company code level. Profit Centers in SAP S/4HANA can be organized hierarchically in Profit Center groups to depict the organization‘s structure. The primary hierarchy is associated with the controlling area and is referred to as the standard hierarchy. There may also be a requirement to assign multiple company codes to a single Profit Center.
-The Profit Center master data is period specific, so the master record has a validity period. It should be possible to create the Profit Center master data using the program created for this specification. These Profit Centers, once loaded into the system, will help with financial consolidation and planning</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>1.Profit Centers must be created and activated through this upload.
-2.Profit Center groups (Hierarchy) should be created prior to executing the upload.</t>
-  </si>
-  <si>
-    <t>dfcdeb53-7837-429c-88df-6b9698ee07a3</t>
-  </si>
-  <si>
-    <t>1.Upload file will be provided in .xls/.txt format with data across the relevant SAP S/4HANA fields
-2.The file should be uploaded into SAP S/4HANA to create Profit Center master data and/or activate
-3.Uploaded data will be validated by downloading and comparing against the input file
-4.Controlling Area -- Must be Defaulted to the Olin’s Controlling Area
-5.Valid From Date – The “Valid From date” of all Profit Centers should be defaulted as per the load file
-6.Valid To Date – The “Valid To Date” of all Profit Centers should be defaulted to "99991231"
-7.Profit Center Group- Parent Hierarchy Node for all Profit Centers. Relevant Profit Center group needs to be identified and manually populated in the Excel file before upload.</t>
-  </si>
-  <si>
     <t> </t>
   </si>
   <si>
-    <t>1ed96bc6-aa39-4659-a54b-6c99f044d147</t>
-  </si>
-  <si>
     <t>Med</t>
   </si>
   <si>
-    <t>81347f68-be7a-4497-a3db-a0c42cfb64a3</t>
-  </si>
-  <si>
-    <t>72a7bb14-da04-4df5-ad10-1a1183778418</t>
-  </si>
-  <si>
-    <t>4550891c-3a59-474c-a929-12a9dc17e562</t>
-  </si>
-  <si>
-    <t>Upload spreadsheet into SAP</t>
-  </si>
-  <si>
-    <t>The Profit Centers in the spreadsheet should be created in SAP with all applicable data in the correct fields</t>
-  </si>
-  <si>
-    <t>Create Profit  center after upload</t>
-  </si>
-  <si>
-    <t>Duplicate Profit Center fails to create as Profit Center already exists</t>
-  </si>
-  <si>
-    <t>File with no Profit Center Group</t>
-  </si>
-  <si>
-    <t>Should error out and Profit Centers should not be created</t>
-  </si>
-  <si>
-    <t>Incorrect Profit Center Group</t>
-  </si>
-  <si>
-    <t>Company Code Omitted</t>
+    <t xml:space="preserve">Set up Customs Management Module </t>
+  </si>
+  <si>
+    <t>Set up configuration for customs declaration, form output and default rules for document printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The purpose of the form is to be able to print the Customs Invoice required by Canadian Customs Authorities for goods being exported into Canada. The exportoring party should should print the invoice. </t>
+  </si>
+  <si>
+    <t>Automate printing of document on a transactional basis for cross-border movement sent to Canada. Allow printing of the Canadian Customs Invoice during export process when sending goods to Canada via customs declarations</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Form to print canadian custom invoice(CCI) required by Canadian Customs Authorities.</t>
+  </si>
+  <si>
+    <t>7c1f1da4-d40f-4f9b-8f32-9a43f781034d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•Canadian Customs form will be generated from GTS
+•Standard global template will be used unless there are requirements for localized forms in local languages 1.Start
+</t>
+  </si>
+  <si>
+    <t>4f9be2e1-1645-4354-84f2-ce82471c5003</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>97bbfa7a-5676-4943-8dc6-adee51a3afc6</t>
+  </si>
+  <si>
+    <t>Print whenever goods are being exported to Canada</t>
+  </si>
+  <si>
+    <t>No additional security requirements. The Standard GTS security objects are sufficient.</t>
+  </si>
+  <si>
+    <t>1.Start
+2.Create Interface Z*Tcode In SFP transaction
+3.Create From Z*TCODE with intercae Z*tcode in SFP transaction.
+4.Give required output field with logic for determining field value.
+5.click on execute to print canadian customs invoice form
+6.END</t>
+  </si>
+  <si>
+    <t>1770b99d-2e12-4073-8b6d-50bb0aea105e</t>
+  </si>
+  <si>
+    <t>a4496e6d-f61e-44f5-b4dc-59e96e6f1071</t>
+  </si>
+  <si>
+    <t>Issue – One material</t>
+  </si>
+  <si>
+    <t>Issue Form correctly printed for one material</t>
+  </si>
+  <si>
+    <t>Issue – Multiple materials</t>
+  </si>
+  <si>
+    <t>Issue Form correctly printed for multiple materials</t>
+  </si>
+  <si>
+    <t>issue – Multiple materials</t>
+  </si>
+  <si>
+    <t>Pending for test data</t>
+  </si>
+  <si>
+    <t>Invoice to be generated in Invoice document automatically in VF01/VF02/VF03 in SAP and Re-print in VF31. 
+Invoice will be issued either Print or Email or through FAX.</t>
+  </si>
+  <si>
+    <t>1.	Customer Master/BP should be present in the system
+2.	Required Configuration for Output type and determination is complete
+3.	Correspondence and associated configuration
+4.	PDF based Forms configuration 
+5.	Printers set up
+6.	Customer Invoices Processed 
+7.	Once invoice is posted, business processes correspondence to print the invoice</t>
+  </si>
+  <si>
+    <t>The Customer Invoice form/Credit Memo form will be trigerred after executing transaction FB12 to request Customer Invoice Correspondence document. The status of the request can be checked using F.64 transaction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The form has to be generated for Customer Invoice and Credit Memos (Document type – “DG” and “DR”). The form will have 2 versions one for US where the headings will be only in English and second for company codes operating in Canada with headings in two languages (English + French). </t>
+  </si>
+  <si>
+    <t>Form to print cutomer invoice and credit memos</t>
+  </si>
+  <si>
+    <t>e974ab65-279e-414a-8694-ecddf2f2282c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data will be extracted from FI-AR Generating the Form. This stardard invoice for will be generated in the defined format below. The form has to be generated for Customer Invoice and Credit Memos (Document type – “DG” and “DR”). The form will have 2 versions one for US where the headings will be only in English and second for company codes operating in Canada with headings in two languages (English + French). So in total 4 forms will be developed English(Invoice and Credit Memo) and English+French (Incoice and Credit Memo). Following are the fields that will be displayed onto the Invoice/Credit Memo main Form:
+1.	Company Logo/address 
+2.	Sold To 
+3.	Bill To 
+4.	Invoice No
+5.	Invoice Date 
+6.	Page 
+7.	Payer Number
+8.	Company Code Currency
+9.	Terms 
+10.	Reference
+11.	Due Date - Due Date (calculate from Baseline date + Payment Terms) 
+12.	Line No 
+13.	Description 
+14.	Net Amount 
+15.	Invoice Total
+16.	Payment Coupn 
+Following fields will be present in the lower part of the Form (Payment Coupon).
+17.	Important Instruction
+18.	Customer Name &amp; Address
+19.	Invoice Date
+20.	Payer Number
+21.	Invoice No
+22.	Amount Due 
+23.	Reference
+24.	Please Remit To information
+25.	Comments
+26.	Footer line with System details source information
+For Credit Memo (DocType: DG), display labels as Document Date, Document number instead of Invoice Number and Invoice Date wherever applicable.
+The Sample of the Invoice Form is attached in the Form Layout Section for English and English+French. The only Change for Credit Memo form will be that the “INVOICE” will be replaced with “CREDIT MEMO” for English Form and “CREDIT MEMO/ NOTE DE CREDIT).
+Logic for populating the line items in the form-
+1.	Document Type DR (Invoice) –
+Fetch records from BSEG table for the document number and BSEG-SHKZG = ‘H’
+2.	Document Type DG (Credit Memo) – 
+Fetch records from BSEG table for the document number and BSEG-SHKZG = ‘S’
+If the number of line items are huge then 1st 8 line items of one Invoice should be printed on the 1st page and then rest can be taken to the next page for better visibility. 
+The Total Invoice amount and the Payment Coupon part of the information should appear only after the last line item of the invoice/credit memo. </t>
+  </si>
+  <si>
+    <t>999ecc94-7e94-4477-bd19-c1539700f5c9</t>
+  </si>
+  <si>
+    <t>80643a1f-b2d1-4a7e-9439-b7bfa7bb799a</t>
+  </si>
+  <si>
+    <t>1.	Customer Master/BP should be present in the system
+2.	Required Configuration for FI-AR is complete
+3.	Correspondence and associated configuration
+4.	PDF based Forms configuration 
+5.	Printers set up
+6.	Customer Invoices Processed 
+7.	Once invoice is posted, business processes correspondence to print the invoice
+8.	Company Codes for which French descriptions should also appear in the form, should be maintained against TVARVC entry Name “ZF005_FRENCH_CC” 
+9.	Logos for different company codes should be of same size because different sizes will disturb the alignment on the form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data will be extracted from FI-AR Generating the Form. This stardard invoice for will be generated in the defined format below. The form has to be generated for Customer Invoice and Credit Memos (Document type – “DG” and “DR”). The form will have 2 versions one for US where the headings will be only in English and second for company codes operating in Canada with headings in two languages (English + French). So in total 4 forms will be developed English(Invoice and Credit Memo) and English+French (Incoice and Credit Memo). Following are the fields that will be displayed onto the Invoice/Credit Memo main Form:
+1.	Company Logo/address 
+2.	Sold To 
+3.	Bill To 
+4.	Invoice No
+5.	Invoice Date 
+6.	Page 
+7.	Payer Number
+8.	Company Code Currency
+9.	Terms 
+10.	Reference
+11.	Due Date - Due Date (calculate from Baseline date + Payment Terms) 
+12.	Line No 
+13.	Description 
+14.	Net Amount 
+15.	Invoice Total
+16.	Payment Coupn 
+Following fields will be present in the lower part of the Form (Payment Coupon).
+17.	Important Instruction
+18.	Customer Name &amp; Address
+19.	Invoice Date
+20.	Payer Number
+21.	Invoice No
+22.	Amount Due 
+23.	Reference
+24.	Please Remit To information
+25.	Comments
+26.	Footer line with System details source information
+For Credit Memo (DocType: DG), display labels as Document Date, Document number instead of Invoice Number and Invoice Date wherever applicable.
+The Sample of the Invoice Form is attached in the Form Layout Section for English and English+French. The only Change for Credit Memo form will be that the “INVOICE” will be replaced with “CREDIT MEMO” for English Form and “CREDIT MEMO/ NOTE DE CREDIT).
+Logic for populating the line items in the form-
+1.	Document Type DR (Invoice) –
+Fetch records from BSEG table for the document number and BSEG-SHKZG = ‘H’
+2.	Document Type DG (Credit Memo) – 
+Fetch records from BSEG table for the document number and BSEG-SHKZG = ‘S’
+If the number of line items are huge then 1st 8 line items of one Invoice should be printed on the 1st page and then rest can be taken to the next page for better visibility. 
+The Total Invoice amount and the Payment Coupon part of the information should appear only after the last line item of the invoice/credit memo. 
+For the English+French form only the heading should be displayed in both English and their translation in French. The sample is attached. Address and Line item details in English only. </t>
+  </si>
+  <si>
+    <t>Access to print the initial collection letter should be limited to Account Receivable Manager, Account Receivable Accountant.</t>
+  </si>
+  <si>
+    <t>In total 4 forms will be developed English(Invoice and Credit Memo) and English+French (Incoice and Credit Memo).</t>
+  </si>
+  <si>
+    <t>The Customer Invoice Form has to be generated as an Invoice or Credit Memo, based on document type (‘DG-Credit Memo’ &amp; ‘DR-Debit Memo’).
+1.	Copy the Interface FI_RFKORD of standard Adobe Form F140_DOCU_EXC_01 to ZAR_INF_CUSTOMER_INVOICE. 
+2.	Create an adobe form ZARF005_CUSTOMER_INVOICE and link it with the interface ZAR_INF_CUSTOMER_INVOICE.
+3.	Then configure the created ZARF005_CUSTOMER_INVOICE against the standard program RFKORD50_PDF in PDF based Forms Configuration.
+4.	In code Initialization fetch the Company Code (BUKRS), Accounting Document No. (BELNR) and Fiscal Year (GJAHR) from the driver program.
+5.	Pseudo code in Code Initialization:
+5.1	SUB_GET_BKPF -Fetch Accounting Document Header data from BKPF table based on entered Company Code (BUKRS), Document Number (BELNR) &amp; Fiscal Year (GJAHR) from LS_HEADER structure (which is copied from standard Interface FI_RFKORD). 
+Pass Company Code (BUKRS), Document number (BELNR) and fiscal year (GJAHR) from driver program to BKPF and fetch the following fields
+BKPF-BUKRS "Company Code
+BKPF-BELNR "Doc No
+BKPF-GJAHR "Fiscal Year
+BKPF-BLDAT "Doc Date
+BKPF-BUDAT "Posting Date
+BKPF-BLART "Doc Type
+BKPF-WAERS "Doc Currency
+BKPF-XBLNR "Reference
+If Document Type BKPF-BLART = ‘DG’, Print ‘Credit Memo’ and if BKPF-BLART = ‘DR’, Print ‘Invoice’
+5.2	SUB_GET_BSEG – Pass Company Code, Document Number &amp; Fiscal Year from the driver program and fetch the following fields from BSEG with KOART ‘D’ (Customer Line) and KOART = ‘S’ (GL Lines)  BSEG-BUKRS "Company Code
+BSEG-BELNR "Doc No
+BSEG-GJAHR "Fiscal year
+BSEG-BUZEI "Line Item
+BSEG-KOART "Customer/GL Line Indicator
+BSEG-DMBTR "Amount in Local currency
+BSEG-WRBTR "Amount in Doc currency
+BSEG-HKONT "GL Account
+BSEG-KUNNR "Customer
+BSEG-ZFBDT "Base Date
+BSEG-ZTERM "Payment Terms
+BSEG-ZBD1T "PT Days
+BSEG-NETDT "Net Due Date
+BSEG-H_BUDAT "Document Date
+BSEG-H_BLDAT "Posting Date
+5.3	SUB_GET_SKAT – Fetch description of each GL from SKAT where SKAT-SAKNR = BSEG-HKONT and KTOPL = T001-KTOPL 
+5.4	SUB_FILL_HEADER –Fill Header details into a Global structure GS_HEAD with details like document date, posting date, local currency, document currency, reference number, Customer &amp; Company Code Address, Payment Terms, Due Date Etc.
+5.5	SUB_GET_TRANSLATIONS-Fill the global fields which has text in English and French Languages from the table ZADT_LABEL_MAINT.
+5.6	SUB_GET_ADDRESS –
+Fetch Company’s address from address table ADRC (text table having address (T005U-Region Text, T005T Country Text) where ADRC-ADDRNUMBER = T001-ADRNR.
+Fetch Company’s address (Remit To) from T049L where BUKRS = BKPF-BUKRS.
+Fetch Company’s address from address table ADRC (text table having address (T005U-Region Text, T005T Country Text) where ADRC-ADDRNUMBER = T049L-ADRNR.
+Fetch customer address from KNA1 where KUNNR = BSEG-KUNNR &amp; ADRC table where ADRC-ADDRNUMBER = KNA1-ADRNR.
+Fetch the region Text from T005U where LAND1 = ADRC-LAND1 and BLAND = ADRC-REGION. Fetch country text from T005T where LAND1 = ADRC-LAND1.
+5.7	SUB_FORMAT_ADDRESS –Format addresses in such a way that if an address field is empty then it will not leave a space and will concatenate the rest of the result.
+5.8	SUB_FILL_ITEMTABLE -Fill item table with details to be displayed in tabular format (Line Number, GL Description and Net Amount (BSEG-DMBTR) in Form with only GL Lines (KOART = ‘S’ from BSEG Table). 
+5.9	FORM SUB_DYNAMIC_LOGO uploads the logo in the form using method “GET_LOGOS” from custom class “ZCL_COMMON_UTILITY”. Input company code, today’s date and form name to this method and it returns logo name as output. Now input the obtained logo name to the method GET_LOGOS_MIME of class ZCL_COMMON_UTILITY (The logos stored in MIME Repository) and it returns the logo.
+6.	Header structure GS_HEAD &amp; Item Table GT_ITEM which are filled in Forms SUB_FILL_HEADER &amp; SUB_FILL_ITEMTABLE to be used to bind to the elements of Adobe Form.
+7.	Apart from GS_HEAD &amp; GT_ITEM mentioned in above point, the following objects are also included in the context area of the Form.
+GV_FRENCH_FLAG: Indictor when ‘X’ Form to be printed in English and French. When ‘‘, Print only in English. This indicator flag is filled based on Company Code.
+Company Codes for which form to be printed in French should be maintained against the TVARVC entry Name “ZF005_FRENCH_CC”
+SFPSY: Standard system fields 
+LOGO: Logo to be displayed on Form Header in Page1
+All the global text fields with multi lingual data from table ZADT_LABEL_MAINT are bound in the form
+8.	Bind the table fields Item Counter, GL Long Description and Amount in local currency with each of the fields of adobe form.
+9.	Execute the form from transaction F.64.</t>
+  </si>
+  <si>
+    <t>253a4101-5c2d-4e29-96e3-4331076b70b7</t>
+  </si>
+  <si>
+    <t>403259ab-d564-4c86-80e5-0e53eed16d9c</t>
+  </si>
+  <si>
+    <t>Enter transaction FB12. Select form as Customer Invoice</t>
+  </si>
+  <si>
+    <t>Form Request should be accepted</t>
+  </si>
+  <si>
+    <t>Invoice Form should be generated in correct format</t>
+  </si>
+  <si>
+    <t>Invoice should be generated in correct format</t>
+  </si>
+  <si>
+    <t>Invoice Form Details should be accurate</t>
+  </si>
+  <si>
+    <t>Invoice Details should be accurate</t>
+  </si>
+  <si>
+    <t>Invoice Form should have correct layout as specified</t>
+  </si>
+  <si>
+    <t>For Credit Memos the required fields like Invoice Date and Invoice Number should be displayed as mentioned above</t>
+  </si>
+  <si>
+    <t>The Invoice Number should be replaced with Document Number and Invoice Date should be replaced by Document Date and Invoice heading to be replaced by “Credit Memo”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +559,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -410,10 +627,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,249 +949,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF51807-B8B4-4457-AEF4-34BF8098CA98}">
-  <dimension ref="A1:BS2"/>
+  <dimension ref="A1:BT3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="36.88671875" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>71</v>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>863</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" t="s">
         <v>75</v>
       </c>
       <c r="F2" t="s">
@@ -989,184 +1210,306 @@
         <v>80</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="O2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="P2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="R2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="S2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
         <v>81</v>
       </c>
-      <c r="T2" t="s">
-        <v>80</v>
-      </c>
       <c r="U2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s">
         <v>82</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" t="s">
         <v>73</v>
       </c>
-      <c r="X2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>80</v>
-      </c>
       <c r="AB2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AE2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AF2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AG2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="AH2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="AI2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AK2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AL2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AM2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AN2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AO2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AP2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AQ2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AR2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AS2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AT2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AU2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AV2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AW2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AX2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>88</v>
       </c>
       <c r="BA2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="BB2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="BC2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="BD2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BE2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BF2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BG2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BH2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="BK2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="BL2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="BM2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="BN2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="BO2" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="BP2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="BQ2" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="BR2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="BS2" t="s">
-        <v>91</v>
+        <v>71</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2203</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+      <c r="T3" t="s">
+        <v>102</v>
+      </c>
+      <c r="W3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>112</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>116</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>119</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>112</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>113</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>114</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>115</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>116</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>118</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>